<commit_message>
fetch resumes from db
</commit_message>
<xml_diff>
--- a/exports/swapnil13/resumes.xlsx
+++ b/exports/swapnil13/resumes.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -431,12 +431,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="19" customWidth="1" min="1" max="1"/>
-    <col width="32" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="33" customWidth="1" min="2" max="2"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
     <col width="50" customWidth="1" min="5" max="5"/>
-    <col width="39" customWidth="1" min="6" max="6"/>
+    <col width="33" customWidth="1" min="6" max="6"/>
     <col width="50" customWidth="1" min="7" max="7"/>
     <col width="50" customWidth="1" min="8" max="8"/>
     <col width="50" customWidth="1" min="9" max="9"/>
@@ -445,7 +445,7 @@
     <col width="10" customWidth="1" min="12" max="12"/>
     <col width="50" customWidth="1" min="13" max="13"/>
     <col width="24" customWidth="1" min="14" max="14"/>
-    <col width="22" customWidth="1" min="15" max="15"/>
+    <col width="19" customWidth="1" min="15" max="15"/>
     <col width="19" customWidth="1" min="16" max="16"/>
     <col width="33" customWidth="1" min="17" max="17"/>
   </cols>
@@ -540,143 +540,125 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>SWAPNIL SHETE</t>
+          <t>PRASHANT KISHORE</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>sheteswapnil13@gmail.com</t>
+          <t>kishore.prashant23@gmail.com</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>9503547253</t>
+          <t>+91-773-976-6918</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr"/>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>www.linkedin.com/in/swapnilshete13</t>
+          <t>https://linkedin.com/in/kishore-prashant23</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>Core Java
-Java 8 Features
-Collections Framework
-Python
-MySQL
-Hibernate/JPA
-React
-Spring Boot
-Spring Security
-Spring Data JPA
-REST APIs
-Data Structures
-DBMS
-Operating Systems
-Computer Networks
-VS code
-IntelliJ
+          <t>Python
+Kubernetes
+MongoDB
+PostgreSQL
+Ruby on Rails
 Postman
-Git
-Supervised &amp; Unsupervised Learning
-Model Evaluation
-Data Preprocessing
-Data Analysis
-Scikit-learn
-Pandas
-NumPy
-Power BI
-Core Python
-Pydantic
-FastAPI
-Django</t>
+Java
+ETL
+Kafka
+GIT
+Unix
+Docker
+AWS
+Azure
+Microservices
+React JS</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Bachelor Of Technology in Artificial Intelligence and Data Science - Vishwakarma Institute Of Information Technology (2022 - 2026); 12th Grade (PCM) - Babuji Avhad Mahavidyalaya, Pathardi (2021 - 2022); 10th Grade - Shri Tilok Jain Vidyalaya, Pathardi (2019 - 2020)</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr"/>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>Modern Lights - AI Powered Ecommerce Platform For Home Decor Products [Spring Boot, Hibernate, MySQL, React, JWT, GenAI, Vercel]: Developed a full-stack e-commerce platform for home decor lighting products. Built backend using Spring Boot with JWT-based security and MySQL.. Integrated GenAI (Gemini Pro) for personalized product recommendations. Created RESTful APIs for seamless frontend-backend communication. Collaborated on React.js frontend and deployed on Vercel.
-AI-Enabled School Management System [FastAPI, Python, MySQL, React, Scikit-learn, Pydantic]: Developed a full-stack school management platform for student registration, attendance, fee management, and academic performance analysis with ML-based predictive insights. Built RESTful APIs using FastAPI, ensured data validation with Pydantic, and integrated frontend using React.</t>
-        </is>
-      </c>
+          <t>Master of Computer Applications - Birla Institute of Technology, Mesra, Ranchi (July 2020); Bachelor of Computer Applications - Birla Institute of Technology, Mesra, Ranchi (July 2017)</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Software Developement Engineer II at Tata 1mg (2025-04 - Present)
+ Developing the next supply chain management application for retail arm of Tata 1mg.
+Lead design discussions, and mentoring junior developers.
+Software Developer (amAIz) at Amdocs Development Center India LLP (2024-02 - 2025-03)
+ Developed FASTAPI based RESTAPIs for amAIz platform and amAIz-SDKs(python package) to be used by internal-external clients.
+Implemented the tenant management and RBAC into the amAIz Application and integrated it with amAIz SDK to enable proper data fencing.
+Integrated Azure API management to enable multiple regions support of Azure OpenAI services and NIM services without having to maintain API keys as configuration as a code.
+Software Developer (Versionless R&amp;D) at Amdocs Development Center India LLP (2023-07 - 2024-02)
+ Developed a learning bot based on Langchain framework to help and mentor new joiners for Amdocs CEP learning using Azure OpenAI LLMs and Embeddings, currently being used by more than 1000+ people.
+Successfully completed a POC for RFP answer generation using Generative AI.
+Software Developer (Telstra Australia) at Amdocs Development Center India LLP (2022-01 - 2023-06)
+ Lead customer meetings for understanding change requests from business and help troubleshooting any issues.
+Implemented a reporting template for stakeholders in bash for sending mails by extracting data from DB, formatted in HTML and CRON timed, for reducing manual monitoring of ETL jobs by 80%.
+Proposed and created a mechanism for re-processing of records(remediation) end-to-end, based on a specific attribute value or for a specific duration.
+Software Engineering Associate (Telstra Australia) at Amdocs Development Center India LLP (2020-09 - 2021-12)
+ Built ETLs that ingested transactional event data from a PostgreSQL database and Utilized Kafka to distribute event streaming datasets to improve processing and ingestion of the data which had approx. 12,000,000 new upserts coming in every day.
+Developed and implemented a logic to extract updates for business entities in PostgreSQL, based on updates to the child tables, even if there is no update in the parent table.
+Software Engineering Intern at Amdocs Development Center India LLP (2020-01 - 2020-05)
+ Created a dashboard for visualization was made using Elastic stack and was set up on Docker to reduce time for tracing of distributed logs generated by micro-services.</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr"/>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>Java 8 New Features - Udemy
-Spring Boot 3
-Spring 6 &amp; Hibernate - Udemy
-Java FullStack Developer - IBM
-Programming In Python - Meta
-Introduction to FastAPI Framework - Duke University</t>
+          <t>AWS Certified Cloud Practitioner
+Hacker Rank: SQL- Intermediate</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
         <is>
-          <t>0 yr</t>
+          <t>5 yrs 3 mos</t>
         </is>
       </c>
       <c r="L2" s="2" t="n">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="M2" s="2" t="inlineStr">
         <is>
-          <t>Candidate lacks the required 2 years of experience.
-The Bachelor of Technology degree in Artificial Intelligence and Data Science is highly relevant for the role
-but it is still in progress (expected completion 2026).
-Candidate has strong foundational skills in Python
-Machine Learning concepts
-SQL (MySQL
-DBMS)
-and Data Analysis (Pandas
-NumPy
-Power BI)
-which are all critical for a Data Scientist role.
-Project experience demonstrates practical application of ML-based predictive insights and data analysis
-directly addressing JD responsibilities.
-Missing the specific 'AWS Machine Learning Foundations' certification mentioned in the JD.</t>
+          <t>Candidate possesses all required skills (Python
+FastAPI)
+with FastAPI explicitly mentioned in their experience descriptions.
+Candidate is significantly overqualified for a 'fresher' role with 5 years and 3 months of relevant experience.</t>
         </is>
       </c>
       <c r="N2" s="2" t="inlineStr">
         <is>
-          <t>2025-11-07 14:43:56</t>
+          <t>2025-11-22 11:43:50</t>
         </is>
       </c>
       <c r="O2" s="2" t="inlineStr">
         <is>
           <t>Python
-Machine Learning
-SQL
-Data Analysis</t>
+FastAPI</t>
         </is>
       </c>
       <c r="P2" s="2" t="inlineStr"/>
       <c r="Q2" s="2" t="inlineStr">
         <is>
-          <t>Core Java
-Java 8 Features
-Collections Framework
-Hibernate/JPA
-React
-Spring Boot
-Spring Security
-Spring Data JPA
-REST APIs
-Data Structures
-Operating Systems
-Computer Networks
-VS code
-IntelliJ
+          <t>Kubernetes
+MongoDB
+PostgreSQL
+Ruby on Rails
 Postman
-Git
-Pydantic
-FastAPI
-Django</t>
+Java
+ETL
+Kafka
+GIT
+Unix
+Docker
+AWS
+Azure
+Microservices
+React JS</t>
         </is>
       </c>
     </row>
@@ -742,17 +724,12 @@
       <c r="H3" s="2" t="inlineStr">
         <is>
           <t>Full Stack Development Engineer at Enphase Energy (2022-07 - Present)
- Designed and implemented an API gateway using Node.js, enabling seamless integration of internal API features into clients’ CRM systems.
-Maintained comprehensive API documentation using OpenAPI and React SPA, improving developer onboarding and usage efficiency.
-Achieved 97% test coverage for public APIs by writing extensive unit tests using Mocha and integration tests via Postman, integrated with CircleCI CI/CD pipelines.
-Developed a PDF converter gateway using Puppeteer to convert browser-rendered quotes to PDFs, asynchronously storing files in AWS S3 with metadata managed in MongoDB.
-Built responsive UI features such as subscription/pricing sections and third-party integrations using React and MaterialUI, enhancing user experience.
-Automated API monitoring dashboards using Dynatrace and Python for log monitoring, resulting in a {{20–30%}} improvement in average API response times measured via Apache JMeter.</t>
+ Designed and implemented an API gateway using Node.js, enabling seamless integration of internal API features into clients’ CRM systems. Maintained comprehensive API documentation using OpenAPI and React SPA, improving developer onboarding and usage efficiency. Achieved 97% test coverage for public APIs by writing extensive unit tests using Mocha and integration tests via Postman, integrated with CircleCI CI/CD pipelines. Developed a PDF converter gateway using Puppeteer to convert browser-rendered quotes to PDFs, asynchronously storing files in AWS S3 with metadata managed in MongoDB. Built responsive UI features such as subscription/pricing sections and third-party integrations using React and MaterialUI, enhancing user experience. Automated API monitoring dashboards using Dynatrace and Python for log monitoring, resulting in a {{20–30%}} improvement in average API response times measured via Apache JMeter.</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>Phonocardiogram (Heart Sound) Processing and Classification [Signal processing, Autocorrelation, Enveloping, Thresholding, Spectrograms, Scalograms, Deep learning, 2D CNN, BiLSTM, LaTeX]: Segmented heart sounds of patients into cardiac cycles using signal processing techniques such as autocorrelation, enveloping, and thresholding. Built 2D representations of signals using Spectrograms and Scalograms, and applied deep learning models like 2D CNN and BiLSTM for classification, achieving an accuracy of 92% with the BiLSTM attention-based model. Authored a detailed Master’s thesis using LaTeX, incorporating complex charts, figures, styles, and references.</t>
+          <t>Phonocardiogram (Heart Sound) Processing and Classification [Signal Processing, Autocorrelation, Enveloping, Thresholding, Spectrograms, Scalograms, 2D CNN, BiLSTM, Deep Learning, LaTeX]: Segmented heart sounds of patients into cardiac cycles using signal processing techniques such as autocorrelation, enveloping, and thresholding. Built 2D representations of signals using Spectrograms and Scalograms, and applied deep learning models like 2D CNN and BiLSTM for classification, achieving an accuracy of 92% with the BiLSTM attention-based model. Authored a detailed Master’s thesis using LaTeX, incorporating complex charts, figures, styles, and references.</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr"/>
@@ -762,33 +739,40 @@
         </is>
       </c>
       <c r="L3" s="2" t="n">
-        <v>69.5</v>
+        <v>60</v>
       </c>
       <c r="M3" s="2" t="inlineStr">
         <is>
-          <t>Outstanding strength in relevant skills: The candidate possesses strong Python and SQL skills
-and significant practical experience in Machine Learning (Deep Learning models) and Data Analysis (Signal processing
-data representation) demonstrated through their academic project.
-Excellent academic background: The B.Tech + M.Tech (Dual Degree) with a minor in Computer Science and Engineering from IIT Kharagpur is a significant asset.
-Exceeds experience requirement: The candidate's 3.33 years of experience surpasses the 2 years required.
-Area for improvement: The candidate does not have the 'AWS Machine Learning Foundations' certification listed.
-Location mismatch: The candidate's location (Bangalore) does not match the job location (Pune).</t>
+          <t>The candidate's 3.33 years of experience significantly exceeds the 'fresher' requirement for this role
+making them overqualified in terms of experience.
+The candidate demonstrates strong proficiency in Python
+which is a key skill for the role
+but FastAPI is a missing skill.
+The candidate possesses a broad range of skills including full-stack development
+cloud (AWS S3)
+containerization (Docker
+Kubernetes)
+CI/CD (Jenkins
+CircleCI)
+and monitoring tools (Dynatrace
+Grafana) which go beyond the stated job description requirements.</t>
         </is>
       </c>
       <c r="N3" s="2" t="inlineStr">
         <is>
-          <t>2025-11-07 15:23:48</t>
+          <t>2025-11-22 11:43:50</t>
         </is>
       </c>
       <c r="O3" s="2" t="inlineStr">
         <is>
-          <t>Python
-MySQL
-Deep learning
-Signal processing</t>
-        </is>
-      </c>
-      <c r="P3" s="2" t="inlineStr"/>
+          <t>Python</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>FastAPI</t>
+        </is>
+      </c>
       <c r="Q3" s="2" t="inlineStr">
         <is>
           <t>JavaScript
@@ -800,6 +784,7 @@
 Express
 HTML
 Node.js
+MySQL
 MongoDB
 Git
 Mocha
@@ -812,21 +797,14 @@
 Dynatrace
 Jenkins
 CircleCI
-Grafana
-Autocorrelation
-Enveloping
-Thresholding
-Spectrograms
-Scalograms
-2D CNN
-BiLSTM</t>
+Grafana</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Sachin Pandey</t>
+          <t>SACHIN PANDEY</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -841,7 +819,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Bengaluru,Karnataka,India</t>
+          <t>Bengaluru, Karnataka, India</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
@@ -852,138 +830,168 @@
       <c r="F4" s="2" t="inlineStr">
         <is>
           <t>Agile Methodology
-Python
+Agentic AI
+AWS
+BERT
+CNN
+Chunking
+Computer Vision
+Deep Learning
+Docker
+Elasticsearch
+ETL
+Fast API
+Function Call
+Generative AI
+GPT Model
+JWT
+Kafka
+Kubernetes
+Langchain
+Langgraph
+Llama
+LLM
+LSTM
 Machine Learning
-Deep Learning
-Natural Language Processing
-LLM
-Generative AI
-Computer Vision
-Prompt Engineering
-RAG
-Langchain
-Agentic AI
-Function Call
-VLLM
-QLoRa
-Llama
-Chunking
-OpenAI
-Langgraph
-Kafka
-FastAPI
-JWT
+MDLSTM
 Mistral 7B
 Mistral Instruct
-GPT
-BERT
+Natural Language Processing
+OCR
+Onnx
+OpenAI
+Prompt Engineering
+Pytorch
+Python
+QLoRa
+RAG
+Semantic Segmentation
 SQL
-CNN
-LSTM
-Onnx
-MDLSTM
-AWS
-PyTorch
 TensorFlow
-Docker
-Kubernetes
-Elasticsearch</t>
+VLLM</t>
         </is>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>B.Tech + M. Tech (Integrated Dual Degree Course) CS + SE - GAUTAM BUDDHA UNIVERSITY (2018)</t>
+          <t>B.Tech + M. Tech (Integrated Dual Degree Cource) CS + SE - GAUTAM BUDDHA UNIVERSITY (2018)</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>Gen AI Engineer at Concentrix (2024-01 - Present)
- Generate strategic documentation by processing meeting notes and GONG call data through an LLM model [Gen AI, Prompt Engineering, RAG, Langchain]. Develop a social listening agent using Langgraph for Linkedin Marketing solution for topic detection, sentiment extraction, and engagement insights, which tracks keywords, competitors, and emerging trends and provides company insight in the form of decks [Agentic AI, Gen AI, Prompt Engineering, Function Call, Machine Learning, Langgraph]. Fine-tuned a Llama model and implemented RAG to develop a Q&amp;A system for tender documents [VLLM, QLoRa, Llama]. Designed and implemented a Multi-Hop RAG system to create structured representations of legal contracts, linking clauses, and amendments using a DataFrame agent for efficient retrieval and analysis [RAG, Chunking, OpenAI, Langchain].
-Data Scientist - II at Mastercard (2021-01 - 2024-01)
- Developed an end-to-end AIOps solution using a streaming architecture for real-time log processing, anomaly detection, and root cause analysis, improving system reliability and operational efficiency [Kafka Machine Learning, Fast API, JWT]. Fine-tuning Mistral 7B Base Model with QLoRa on transaction data. Filled a patent for Transaction classification model building and development using LLM. Used Mistral Instruct to extract entities with RAG [Gen AI Based]. Used the GPT model from OpenAI and the Langchain prompt template to automate the labeling process [Gen AI Based]. Solved Financial Institute Transaction categorization problem using the BERT Model with F1-Score 0.86 [LLM Based]. Extraction of Name, Address Account, and Card No for PII Scrubbing process. Entity Extraction model using BERT model with F1 Score of 0.83 [LLM Based]. Executed Proof of Concepts (PoCs) using cutting-edge algorithms based on research. Identification of streaming transactions. Fine-tuned T5 model for Entity Extraction and Transaction Classification tasks both with few-shot learning [Gen AI Based]. Optimized models using Onnx, which reduced 25% of parameters and improved inferencing time [Model Optimization]. Responsible for performing ETL operations for data preparation using SQL operations [ETL].
-Data Scientist at Arya (2020-01 - 2021-01)
- Automated the Insurance underwriting process using deep learning (hybrid model CNN and LSTM) with Precision 0.94 Recall 0.89. Built an Early/fraud claims during underwriting within 3 year span period with Precision 0.67 Recall 0.71. Built an ICD (International Classification of Diseases) Classifier model using BERT and Elasticsearch to find the ICD number of diagnosis report with accuracy of 85%. Extracted insights after advance analysis of insurance data.
-Data Scientist at Unifynd Technologies (2019-01 - 2020-01)
- Built a Churn Prediction model for user onboarding with their drop-off score with an accuracy of 74%. Set up an analytical pipeline for Campaign disposition analysis.
-Data Scientist at CRDR Infotech Pvt. Ltd (2018-01 - 2019-01)
- Built a Cheque Truncation System using semantic segmentation. Included Signet signature verification module which gives an accuracy of 87% and OCR-based MDLSTM for handwritten form recognition Accuracy 79%.</t>
+          <t>Gen AI Engineer at Concentrix ( - Present)
+ Generate strategic documentation by processing meeting notes and GONG call data through an LLM model [Gen AI, Prompt Engineering, RAG, Langchain]
+Develop a social listening agent using Langgraph for Linkedin Marketing solution for topic detection, sentiment extraction, and engagement insights. Which tracks keywords, competitors, and emerging trends and provides company insight in the form of decks. [Agentic AI, Gen AI, Prompt Engineering, Function Call, Machine Learning, Langgraph]
+Fine-tuned a Llama model and implemented RAG to develop a Q&amp;A system for tender documents [VLLM, QLoRa, Llama].
+Designed and implemented a Multi-Hop RAG system to create structured representations of legal contracts, linking clauses, and amendments using a DataFrame agent for efficient retrieval and analysis. [RAG, Chunking, OpenAI, Langchain]
+Data Scientist - II at Mastercard ( - )
+ Developed an end-to-end AIOps solution using a streaming architecture for real-time log processing, anomaly detection, and root cause analysis, improving system reliability and operational efficiency. [Kafka Machine Learning, Fast API, JWT]
+Fine-tuning Mistral 7B Base Model with QLoRa on transaction data
+Filled a patent for Transaction classification model building and development using LLM
+Use Mistral Instruct to extract the entity with RAG [Gen AI Based]
+Use the GPT model from OpenAI and the Langchain prompt template to automate the labeling process [Gen AI Based]
+Solved Financial Institute Transaction categorization problem using the BERT Model with F1- Score 0.86 [LLM Based]
+Extraction of Name, Address Account, and Card No for PII Scrubbing process
+Entity Extraction model using BERT model with F1 Score of 0.83 [LLM Based]
+Data Scientist at Arya ( - )
+ Executed Proof of Concepts (PoCs) using cutting-edge algorithms based on research
+Identification of streaming transactions
+Fine-tuned T5 model for Entity Extraction and Transaction Classification tasks both with few-shot learning [Gen AI Based]
+To further optimize the model use Onnx for optimization which drops 25% of parameters and improves inferencing time [Model Optimization]
+Responsible for performing ETL operations for data preparation using SQL operations [ETL]
+Automated the Insurance underwriting process using deep learning (hybrid model CNN and LSTM) with Precision 0.94 Recall 0.89
+Build an Early/fraud claims during underwriting within 3 year span period with Precision 0.67 Recall 0.71
+Build an ICD (International Classification of Diseases) Classifier model using BERT and elasticsearch to find the ICD number of diagnosis report with accuracy of 85%
+Extract insights after advance analysis of insurance data
+Data Scientist at Unifynd Technologies ( - )
+ Build a Churn Prediction model for user onboarding with their drop-off score with an accuracy of 74%.
+Set up an analytical pipeline for Campaign disposition analysis.
+Data Scientist at CRDR Infotech Pvt. Ltd ( - )
+ Build a Cheque Truncation System using semantic segmentation. Include Signet signature verification module which gives an accuracy of 87% and OCR-based MDLSTM for handwritten form recognition Accuracy 79%.</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr"/>
       <c r="J4" s="2" t="inlineStr"/>
       <c r="K4" s="2" t="inlineStr">
         <is>
-          <t>7 yrs 10 mos</t>
+          <t>0 yr</t>
         </is>
       </c>
       <c r="L4" s="2" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="M4" s="2" t="inlineStr">
         <is>
-          <t>Excellent match for required skills
-experience
-education
-and responsibilities.
-The candidate's extensive experience as a Data Scientist and Gen AI Engineer
-with strong proficiency in Machine Learning
+          <t>All required skills (Python
+FastAPI) are present in the candidate's resume.
+The candidate possesses a wealth of advanced skills and experience in Machine Learning
 Deep Learning
-and Generative AI
-highly exceeds the job description's requirements.
-Missing the specific 'AWS Machine Learning Foundations' certification.
-Candidate's current location (Bengaluru) does not match the job location (Pune).</t>
+Natural Language Processing
+and Generative AI (including LLMs
+RAG
+Langchain
+Prompt Engineering
+MLOps
+AWS
+Docker
+Kubernetes). This extensive background significantly exceeds the requirements for a 'fresher' Software Engineer role.
+There is a notable discrepancy: the 'total_experience_years' in the resume JSON is '0 yr'
+while the detailed 'experience' section clearly outlines multiple professional roles spanning several years. Based on the explicit instruction and the provided 'total_experience_years'
+the experience was scored as a perfect match for a 'fresher' position. However
+the candidate's actual work history suggests they are highly experienced and likely overqualified for this specific role.</t>
         </is>
       </c>
       <c r="N4" s="2" t="inlineStr">
         <is>
-          <t>2025-11-07 15:23:48</t>
+          <t>2025-11-22 11:43:50</t>
         </is>
       </c>
       <c r="O4" s="2" t="inlineStr">
         <is>
           <t>Python
-Machine Learning
-SQL
-Data Analysis</t>
+FastAPI</t>
         </is>
       </c>
       <c r="P4" s="2" t="inlineStr"/>
       <c r="Q4" s="2" t="inlineStr">
         <is>
           <t>Agile Methodology
+Agentic AI
+AWS
+BERT
+CNN
+Chunking
+Computer Vision
 Deep Learning
-Natural Language Processing
+Docker
+Elasticsearch
+ETL
+Function Call
+Generative AI
+GPT Model
+JWT
+Kafka
+Kubernetes
+Langchain
+Langgraph
+Llama
 LLM
-Generative AI
-Computer Vision
-Prompt Engineering
-RAG
-Langchain
-Agentic AI
-Function Call
-VLLM
-QLoRa
-Llama
-Chunking
-OpenAI
-Langgraph
-Kafka
-FastAPI
-JWT
+LSTM
+Machine Learning
+MDLSTM
 Mistral 7B
 Mistral Instruct
-GPT
-BERT
-CNN
-LSTM
+Natural Language Processing
+OCR
 Onnx
-MDLSTM
-AWS
-PyTorch
+OpenAI
+Prompt Engineering
+Pytorch
+QLoRa
+RAG
+Semantic Segmentation
+SQL
 TensorFlow
-Docker
-Kubernetes
-Elasticsearch</t>
+VLLM</t>
         </is>
       </c>
     </row>
@@ -1013,10 +1021,7 @@
           <t>https://www.linkedin.com/in/sakshikusmude-2bb57525a/
 https://github.com/sakshikusmude
 https://www.hackerrank.com/sakshikusmude99
-https://sakshikusmude.github.io/portfolio
-https://www.credly.com/badges/5f85d860-1c5e-4de6-8233-1306c5b8646d/public_url
-https://www.credly.com/badges/18da67d1-bd27-4b1b-a0c6-18705990d1f9/public_url
-https://www.credly.com/badges/c09ba381-3d1e-452a-856f-449c2b17a1db/public_url</t>
+https://sakshikusmude.github.io/portfolio</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -1028,28 +1033,14 @@
 DBMS
 UI/UX designing
 Web Development
+Java
 Python
-Flask
-CNN
-OpenCV
-HTML
-CSS
-Bootstrap
-NLP
-AI Chatbot
-Kotlin
-SQLite
-Firebase
-Data Analysis
-Figma
-Wireframing
-Prototyping
-Java
 C
 C++
 SQL
 VS Code
 Android Studio
+Flask
 Postman
 Intellij Idea
 Tableau
@@ -1057,8 +1048,12 @@
 z/OS
 GitHub
 ReactJS
+Figma
 NodeJS
-Git</t>
+Git
+Data Analysis
+Wireframing
+Prototyping</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
@@ -1078,7 +1073,7 @@
         <is>
           <t>Tuberculosis Detection System [Python, Flask, CNN, OpenCV, HTML, CSS, Bootstrap]: Built a Flask-based web app to detect TB from chest X-rays using a CNN model with over 95% accuracy. Integrated OpenCV for preprocessing and deployed a responsive UI using HTML/CSS and Bootstrap.
 Medical Tourism with Chatbot Integration [Flask, Python, NLP, AI Chatbot]: Integrated an AI-powered chatbot to help patients find the best medical services.
-WorthUnzip [Kotlin, SQLite, Firebase]: Developed an Android app to manage and analyze assets, converting physical assets to digital format and calculating their total value.</t>
+WorthUnzip [Kotlin, SQLite, Firebase, Android]: Developed an Android app to manage and analyze assets, converting physical assets to digital format and calculating their total value.</t>
         </is>
       </c>
       <c r="J5" s="2" t="inlineStr">
@@ -1096,67 +1091,48 @@
         </is>
       </c>
       <c r="L5" s="2" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="M5" s="2" t="inlineStr">
         <is>
-          <t>The candidate demonstrates an excellent match across all weighted criteria including skills
-education
-responsibilities
-certifications
-and location.
-Strong practical experience in building ML models (CNN for TB detection
-AI chatbot) and data analysis through projects and a Data Science internship.
-Key skills like Python
-Machine Learning
-SQL
-and Data Analysis are all present.
-The candidate's total professional experience (0.58 years) is significantly less than the 2 years required by the job description. However
-this field has a weight of 0.0
-so it does not affect the overall score.</t>
+          <t>Candidate has a strong foundation in Python and related machine learning/data science concepts
+demonstrated through projects.
+The candidate's 7 months of experience aligns well with a 'fresher' requirement.
+A key missing skill is FastAPI
+which is specified in the job description.</t>
         </is>
       </c>
       <c r="N5" s="2" t="inlineStr">
         <is>
-          <t>2025-11-07 15:23:48</t>
+          <t>2025-11-22 11:43:50</t>
         </is>
       </c>
       <c r="O5" s="2" t="inlineStr">
         <is>
-          <t>Python
-Machine Learning
-SQL
-Data Analysis</t>
-        </is>
-      </c>
-      <c r="P5" s="2" t="inlineStr"/>
+          <t>Python</t>
+        </is>
+      </c>
+      <c r="P5" s="2" t="inlineStr">
+        <is>
+          <t>FastAPI</t>
+        </is>
+      </c>
       <c r="Q5" s="2" t="inlineStr">
         <is>
-          <t>Data Science
+          <t>Machine Learning
+Data Science
 Data Structures &amp; Algorithms
 OOPS Concept
 DBMS
 UI/UX designing
 Web Development
-Flask
-CNN
-OpenCV
-HTML
-CSS
-Bootstrap
-NLP
-AI Chatbot
-Kotlin
-SQLite
-Firebase
-Figma
-Wireframing
-Prototyping
 Java
 C
 C++
+SQL
 VS Code
 Android Studio
+Flask
 Postman
 Intellij Idea
 Tableau
@@ -1164,152 +1140,12 @@
 z/OS
 GitHub
 ReactJS
+Figma
 NodeJS
-Git</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>SWAPNIL SHETE</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>sheteswapnil13@gmail.com</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>9503547253</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr"/>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/swapnilshete13</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>Core Java
-Java 8 Features
-Collections Framework
-Python
-Spring Boot
-Spring Security
-Spring Data JPA
-REST APIs
-React
-MySQL
-Hibernate/JPA
-Data Structures
-DBMS
-Operating Systems
-Computer Networks
-VS code
-IntelliJ
-Postman
 Git
-Supervised Learning
-Unsupervised Learning
-Model Evaluation
-Data Preprocessing
 Data Analysis
-Scikit-learn
-Pandas
-NumPy
-Power BI
-Core Python
-Pydantic
-FastAPI
-Django</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>Bachelor Of Technology in Artificial Intelligence and Data Science - Vishwakarma Institute Of Information Technology (2026); 12th Grade (PCM) - Babuji Avhad Mahavidyalaya, Pathardi (2022); 10th Grade - Shri Tilok Jain Vidyalaya, Pathardi (2020)</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="inlineStr"/>
-      <c r="I6" s="2" t="inlineStr">
-        <is>
-          <t>Modern Lights - AI Powered Ecommerce Platform For Home Decor Products [Spring Boot, Hibernate, MySQL, React, JWT, GenAI, Vercel, Gemini Pro]: Developed a full-stack e-commerce platform for home decor lighting products. Built backend using Spring Boot with JWT- based security and MySQL. Integrated GenAI (Gemini Pro) for personalized product recommendations. Created RESTful APIs for seamless frontend- backend communication. Collaborated on React.js frontend and deployed on Vercel.
-AI-Enabled School Management System [FastAPI, Python, MySQL, React, Scikit-learn, Pydantic, ML]: Developed a full-stack school management platform for student registration, attendance, fee management, and academic performance analysis with ML-based predictive insights. Built RESTful APIs using FastAPI, ensured data validation with Pydantic, and integrated frontend using React.</t>
-        </is>
-      </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>Java 8 New Features - Udemy
-Spring Boot 3
-Spring 6 &amp; Hibernate - Udemy
-Java FullStack Developer - IBM
-Programming In Python - Meta
-Introduction to FastAPI Framework - Duke University</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="inlineStr">
-        <is>
-          <t>0 yr</t>
-        </is>
-      </c>
-      <c r="L6" s="2" t="n">
-        <v>69</v>
-      </c>
-      <c r="M6" s="2" t="inlineStr">
-        <is>
-          <t>Candidate demonstrates strong foundational skills in Python
-Machine Learning
-SQL
-and Data Analysis
-which are all key requirements for the role.
-Projects showcase practical application of AI/ML concepts
-including building predictive models and data analysis
-directly addressing the responsibilities.
-The 'Bachelor Of Technology in Artificial Intelligence and Data Science' degree is highly relevant and a strong asset for a Data Scientist position.
-Candidate currently has 0 years of experience
-falling significantly short of the required 2 years.
-Lacks the specific 'AWS Machine Learning Foundations' certification mentioned in the job description.
-Candidate's location is not specified
-which is a mismatch for the 'Pune' requirement.</t>
-        </is>
-      </c>
-      <c r="N6" s="2" t="inlineStr">
-        <is>
-          <t>2025-11-07 15:23:48</t>
-        </is>
-      </c>
-      <c r="O6" s="2" t="inlineStr">
-        <is>
-          <t>Python
-Machine Learning
-SQL
-Data Analysis</t>
-        </is>
-      </c>
-      <c r="P6" s="2" t="inlineStr"/>
-      <c r="Q6" s="2" t="inlineStr">
-        <is>
-          <t>Core Java
-Java 8 Features
-Collections Framework
-Spring Boot
-Spring Security
-Spring Data JPA
-REST APIs
-React
-Hibernate/JPA
-Data Structures
-Operating Systems
-Computer Networks
-VS code
-IntelliJ
-Postman
-Git
-Pydantic
-FastAPI
-Django</t>
+Wireframing
+Prototyping</t>
         </is>
       </c>
     </row>

</xml_diff>